<commit_message>
fixed fetch of data, removed * and added sample outputs
</commit_message>
<xml_diff>
--- a/excel data extraction/TravelRestrictionstravel4.xlsx
+++ b/excel data extraction/TravelRestrictionstravel4.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{CF796EC7-F1E4-4893-B67D-2D97719A10EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Travel Restrictions - travel4" sheetId="1" r:id="rId1"/>
@@ -9515,7 +9515,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -10352,10 +10352,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K291"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10408,7 +10410,7 @@
         <v>9.7869519999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -10476,7 +10478,7 @@
         <v>60.154490000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -10502,7 +10504,7 @@
         <v>20220506</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -10528,7 +10530,7 @@
         <v>20220317</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -10554,7 +10556,7 @@
         <v>20200729</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -10580,7 +10582,7 @@
         <v>20220617</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -10609,7 +10611,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -10649,7 +10651,7 @@
         <v>-80.408976999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -10675,7 +10677,7 @@
         <v>20220830</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -10701,7 +10703,7 @@
         <v>20220830</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -10727,7 +10729,7 @@
         <v>20220512</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -10784,7 +10786,7 @@
         <v>-12.242967</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -10836,7 +10838,7 @@
         <v>20220923</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -10879,7 +10881,7 @@
         <v>37.776940000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -10905,7 +10907,7 @@
         <v>20220616</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -10945,7 +10947,7 @@
         <v>0.19478699999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -10971,7 +10973,7 @@
         <v>20220619</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -11011,7 +11013,7 @@
         <v>-21.46322</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -11037,7 +11039,7 @@
         <v>20220801</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -11063,7 +11065,7 @@
         <v>20220926</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -11089,7 +11091,7 @@
         <v>20220816</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>136</v>
       </c>
@@ -11115,7 +11117,7 @@
         <v>20220706</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -11141,7 +11143,7 @@
         <v>20220822</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -11195,7 +11197,7 @@
         <v>15.668231</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>155</v>
       </c>
@@ -11221,7 +11223,7 @@
         <v>20220429</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -11247,7 +11249,7 @@
         <v>20220622</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -11273,7 +11275,7 @@
         <v>20220531</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>169</v>
       </c>
@@ -11313,7 +11315,7 @@
         <v>-54.421104999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>176</v>
       </c>
@@ -11342,7 +11344,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>181</v>
       </c>
@@ -11368,7 +11370,7 @@
         <v>20220715</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -11394,7 +11396,7 @@
         <v>20220915</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>191</v>
       </c>
@@ -11420,7 +11422,7 @@
         <v>20220921</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>196</v>
       </c>
@@ -11446,7 +11448,7 @@
         <v>20220616</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>200</v>
       </c>
@@ -11472,7 +11474,7 @@
         <v>20220824</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>205</v>
       </c>
@@ -11498,7 +11500,7 @@
         <v>20220810</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>210</v>
       </c>
@@ -11524,7 +11526,7 @@
         <v>20220802</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>215</v>
       </c>
@@ -11567,7 +11569,7 @@
         <v>28.283759</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>222</v>
       </c>
@@ -11593,7 +11595,7 @@
         <v>20220826</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>227</v>
       </c>
@@ -11619,7 +11621,7 @@
         <v>20220902</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>231</v>
       </c>
@@ -11645,7 +11647,7 @@
         <v>20210823</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>236</v>
       </c>
@@ -11685,7 +11687,7 @@
         <v>-7.4023700000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>243</v>
       </c>
@@ -11714,7 +11716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>247</v>
       </c>
@@ -11796,7 +11798,7 @@
         <v>-12.18439</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>260</v>
       </c>
@@ -11822,7 +11824,7 @@
         <v>20220105</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>265</v>
       </c>
@@ -11848,7 +11850,7 @@
         <v>20220613</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>270</v>
       </c>
@@ -11874,7 +11876,7 @@
         <v>20220408</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>275</v>
       </c>
@@ -11900,7 +11902,7 @@
         <v>20220914</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>280</v>
       </c>
@@ -11926,7 +11928,7 @@
         <v>20220405</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>285</v>
       </c>
@@ -11952,7 +11954,7 @@
         <v>20220701</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>290</v>
       </c>
@@ -11981,7 +11983,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>295</v>
       </c>
@@ -12007,7 +12009,7 @@
         <v>20220722</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>300</v>
       </c>
@@ -12033,7 +12035,7 @@
         <v>20220622</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>304</v>
       </c>
@@ -12059,7 +12061,7 @@
         <v>20220922</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>308</v>
       </c>
@@ -12099,7 +12101,7 @@
         <v>35.018129999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>313</v>
       </c>
@@ -12125,7 +12127,7 @@
         <v>20200803</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>318</v>
       </c>
@@ -12151,7 +12153,7 @@
         <v>20220824</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>322</v>
       </c>
@@ -12180,7 +12182,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>326</v>
       </c>
@@ -12206,7 +12208,7 @@
         <v>20220918</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>331</v>
       </c>
@@ -12235,7 +12237,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>336</v>
       </c>
@@ -12261,7 +12263,7 @@
         <v>20220809</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>341</v>
       </c>
@@ -12290,7 +12292,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>346</v>
       </c>
@@ -12316,7 +12318,7 @@
         <v>20220620</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>351</v>
       </c>
@@ -12342,7 +12344,7 @@
         <v>20220822</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>355</v>
       </c>
@@ -12368,7 +12370,7 @@
         <v>20220407</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>360</v>
       </c>
@@ -12394,7 +12396,7 @@
         <v>20220412</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>364</v>
       </c>
@@ -12423,7 +12425,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>368</v>
       </c>
@@ -12449,7 +12451,7 @@
         <v>20220404</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>372</v>
       </c>
@@ -12489,7 +12491,7 @@
         <v>-22.364861999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>377</v>
       </c>
@@ -12515,7 +12517,7 @@
         <v>20201027</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>382</v>
       </c>
@@ -12541,7 +12543,7 @@
         <v>20220707</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>387</v>
       </c>
@@ -12567,7 +12569,7 @@
         <v>20201008</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>392</v>
       </c>
@@ -12596,7 +12598,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>397</v>
       </c>
@@ -12625,7 +12627,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>402</v>
       </c>
@@ -12651,7 +12653,7 @@
         <v>20220921</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>406</v>
       </c>
@@ -12677,7 +12679,7 @@
         <v>20220812</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>410</v>
       </c>
@@ -12717,7 +12719,7 @@
         <v>-49.605893000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>415</v>
       </c>
@@ -12746,7 +12748,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>420</v>
       </c>
@@ -12772,7 +12774,7 @@
         <v>20220215</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>425</v>
       </c>
@@ -12798,7 +12800,7 @@
         <v>20211129</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>430</v>
       </c>
@@ -12824,7 +12826,7 @@
         <v>20220616</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>434</v>
       </c>
@@ -12850,7 +12852,7 @@
         <v>20220921</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>438</v>
       </c>
@@ -12876,7 +12878,7 @@
         <v>20220606</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>443</v>
       </c>
@@ -12919,7 +12921,7 @@
         <v>-11.579769000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>448</v>
       </c>
@@ -12945,7 +12947,7 @@
         <v>20220921</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>452</v>
       </c>
@@ -12971,7 +12973,7 @@
         <v>20210326</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>457</v>
       </c>
@@ -12997,7 +12999,7 @@
         <v>20220809</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>461</v>
       </c>
@@ -13023,7 +13025,7 @@
         <v>20220812</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>465</v>
       </c>
@@ -13049,7 +13051,7 @@
         <v>20200526</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>470</v>
       </c>
@@ -13089,7 +13091,7 @@
         <v>49.455675999999997</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>476</v>
       </c>
@@ -13115,7 +13117,7 @@
         <v>20220317</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>480</v>
       </c>
@@ -13141,7 +13143,7 @@
         <v>20220221</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>485</v>
       </c>
@@ -13170,7 +13172,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>489</v>
       </c>
@@ -13241,7 +13243,7 @@
         <v>41.903447999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>500</v>
       </c>
@@ -13267,7 +13269,7 @@
         <v>20220505</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>505</v>
       </c>
@@ -13310,7 +13312,7 @@
         <v>0.80708599999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>510</v>
       </c>
@@ -13336,7 +13338,7 @@
         <v>20220922</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>514</v>
       </c>
@@ -13376,7 +13378,7 @@
         <v>4.7601509999999996</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>520</v>
       </c>
@@ -13402,7 +13404,7 @@
         <v>20220518</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>524</v>
       </c>
@@ -13428,7 +13430,7 @@
         <v>20220718</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>529</v>
       </c>
@@ -13454,7 +13456,7 @@
         <v>20210222</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>533</v>
       </c>
@@ -13480,7 +13482,7 @@
         <v>20220405</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>537</v>
       </c>
@@ -13523,7 +13525,7 @@
         <v>54.228634</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>543</v>
       </c>
@@ -13549,7 +13551,7 @@
         <v>20220526</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>548</v>
       </c>
@@ -13578,7 +13580,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>552</v>
       </c>
@@ -13618,7 +13620,7 @@
         <v>34.554501000000002</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>559</v>
       </c>
@@ -13686,7 +13688,7 @@
         <v>16.729126999999998</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>568</v>
       </c>
@@ -13726,7 +13728,7 @@
         <v>-17.055056</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>573</v>
       </c>
@@ -13752,7 +13754,7 @@
         <v>20220608</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>578</v>
       </c>
@@ -13792,7 +13794,7 @@
         <v>6.4785459999999997</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>583</v>
       </c>
@@ -13818,7 +13820,7 @@
         <v>20220801</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>587</v>
       </c>
@@ -13858,7 +13860,7 @@
         <v>45.076155999999997</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>593</v>
       </c>
@@ -13884,7 +13886,7 @@
         <v>20220512</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>597</v>
       </c>
@@ -13910,7 +13912,7 @@
         <v>20220505</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>601</v>
       </c>
@@ -13936,7 +13938,7 @@
         <v>20220810</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>605</v>
       </c>
@@ -13962,7 +13964,7 @@
         <v>20220922</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>609</v>
       </c>
@@ -13988,7 +13990,7 @@
         <v>20220411</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>614</v>
       </c>
@@ -14028,7 +14030,7 @@
         <v>37.241641999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>620</v>
       </c>
@@ -14054,7 +14056,7 @@
         <v>20220711</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>625</v>
       </c>
@@ -14080,7 +14082,7 @@
         <v>20220225</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>630</v>
       </c>
@@ -14106,7 +14108,7 @@
         <v>20220922</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>634</v>
       </c>
@@ -14132,7 +14134,7 @@
         <v>20220923</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>638</v>
       </c>
@@ -14158,7 +14160,7 @@
         <v>20220921</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>642</v>
       </c>
@@ -14184,7 +14186,7 @@
         <v>20220906</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>647</v>
       </c>
@@ -14224,7 +14226,7 @@
         <v>32.736569000000003</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>652</v>
       </c>
@@ -14250,7 +14252,7 @@
         <v>20220615</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>657</v>
       </c>
@@ -14279,7 +14281,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>661</v>
       </c>
@@ -14305,7 +14307,7 @@
         <v>20220708</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>666</v>
       </c>
@@ -14331,7 +14333,7 @@
         <v>20220923</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>670</v>
       </c>
@@ -14360,7 +14362,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>674</v>
       </c>
@@ -14386,7 +14388,7 @@
         <v>20220922</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>678</v>
       </c>
@@ -14412,7 +14414,7 @@
         <v>20220812</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>682</v>
       </c>
@@ -14438,7 +14440,7 @@
         <v>20220411</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>686</v>
       </c>
@@ -14464,7 +14466,7 @@
         <v>20220701</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>690</v>
       </c>
@@ -14490,7 +14492,7 @@
         <v>20220812</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>694</v>
       </c>
@@ -14516,7 +14518,7 @@
         <v>20220505</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>698</v>
       </c>
@@ -14556,7 +14558,7 @@
         <v>28.209427999999999</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>703</v>
       </c>
@@ -14582,7 +14584,7 @@
         <v>20220826</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>707</v>
       </c>
@@ -14608,7 +14610,7 @@
         <v>20220314</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>712</v>
       </c>
@@ -14634,7 +14636,7 @@
         <v>20220729</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>717</v>
       </c>
@@ -14660,7 +14662,7 @@
         <v>20220711</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>721</v>
       </c>
@@ -14686,7 +14688,7 @@
         <v>20220720</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>725</v>
       </c>
@@ -14712,7 +14714,7 @@
         <v>20220902</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>729</v>
       </c>
@@ -14738,7 +14740,7 @@
         <v>20220817</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>733</v>
       </c>
@@ -14764,7 +14766,7 @@
         <v>20220826</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>737</v>
       </c>
@@ -14804,7 +14806,7 @@
         <v>18.401927000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>742</v>
       </c>
@@ -14830,7 +14832,7 @@
         <v>20220706</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>746</v>
       </c>
@@ -14856,7 +14858,7 @@
         <v>20220920</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>750</v>
       </c>
@@ -14882,7 +14884,7 @@
         <v>20220519</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>755</v>
       </c>
@@ -14911,7 +14913,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>759</v>
       </c>
@@ -14937,7 +14939,7 @@
         <v>20210727</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>764</v>
       </c>
@@ -14963,7 +14965,7 @@
         <v>20220425</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>769</v>
       </c>
@@ -14989,7 +14991,7 @@
         <v>20220819</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>774</v>
       </c>
@@ -15029,7 +15031,7 @@
         <v>-29.032574</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>781</v>
       </c>
@@ -15055,7 +15057,7 @@
         <v>20220503</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>786</v>
       </c>
@@ -15081,7 +15083,7 @@
         <v>20200703</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>791</v>
       </c>
@@ -15110,7 +15112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>795</v>
       </c>
@@ -15139,7 +15141,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>799</v>
       </c>
@@ -15165,7 +15167,7 @@
         <v>20220916</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>804</v>
       </c>
@@ -15205,7 +15207,7 @@
         <v>5.8873620000000004</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>810</v>
       </c>
@@ -15237,7 +15239,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>816</v>
       </c>
@@ -15280,7 +15282,7 @@
         <v>16.834463</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>823</v>
       </c>
@@ -15306,7 +15308,7 @@
         <v>20220609</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>828</v>
       </c>
@@ -15332,7 +15334,7 @@
         <v>20220902</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>832</v>
       </c>
@@ -15358,7 +15360,7 @@
         <v>20220819</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>836</v>
       </c>
@@ -15384,7 +15386,7 @@
         <v>20220823</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>841</v>
       </c>
@@ -15410,7 +15412,7 @@
         <v>20220923</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>845</v>
       </c>
@@ -15436,7 +15438,7 @@
         <v>20220923</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>848</v>
       </c>
@@ -15462,7 +15464,7 @@
         <v>20201203</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>853</v>
       </c>
@@ -15491,7 +15493,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>857</v>
       </c>
@@ -15520,7 +15522,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>861</v>
       </c>
@@ -15549,7 +15551,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>866</v>
       </c>
@@ -15575,7 +15577,7 @@
         <v>20220812</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>870</v>
       </c>
@@ -15604,7 +15606,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>874</v>
       </c>
@@ -15630,7 +15632,7 @@
         <v>20220825</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>878</v>
       </c>
@@ -15659,7 +15661,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>882</v>
       </c>
@@ -15685,7 +15687,7 @@
         <v>20220622</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>886</v>
       </c>
@@ -15714,7 +15716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>890</v>
       </c>
@@ -15740,7 +15742,7 @@
         <v>20220824</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>894</v>
       </c>
@@ -15769,7 +15771,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>898</v>
       </c>
@@ -15795,7 +15797,7 @@
         <v>20220907</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>902</v>
       </c>
@@ -15824,7 +15826,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>906</v>
       </c>
@@ -15850,7 +15852,7 @@
         <v>20220812</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>910</v>
       </c>
@@ -15876,7 +15878,7 @@
         <v>20220920</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>914</v>
       </c>
@@ -15902,7 +15904,7 @@
         <v>20220811</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>919</v>
       </c>
@@ -15928,7 +15930,7 @@
         <v>20220512</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>923</v>
       </c>
@@ -15954,7 +15956,7 @@
         <v>20220503</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>927</v>
       </c>
@@ -15994,7 +15996,7 @@
         <v>15.110537000000001</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>933</v>
       </c>
@@ -16034,7 +16036,7 @@
         <v>25.745757000000001</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>939</v>
       </c>
@@ -16060,7 +16062,7 @@
         <v>20220725</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>944</v>
       </c>
@@ -16086,7 +16088,7 @@
         <v>20220831</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>949</v>
       </c>
@@ -16115,7 +16117,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>954</v>
       </c>
@@ -16141,7 +16143,7 @@
         <v>20220824</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>958</v>
       </c>
@@ -16167,7 +16169,7 @@
         <v>20220622</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>961</v>
       </c>
@@ -16193,7 +16195,7 @@
         <v>20211104</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>966</v>
       </c>
@@ -16219,7 +16221,7 @@
         <v>20220920</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>970</v>
       </c>
@@ -16248,7 +16250,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>974</v>
       </c>
@@ -16274,7 +16276,7 @@
         <v>20220909</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>979</v>
       </c>
@@ -16303,7 +16305,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>984</v>
       </c>
@@ -16343,7 +16345,7 @@
         <v>-54.378486000000002</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>990</v>
       </c>
@@ -16383,7 +16385,7 @@
         <v>31.739991</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>996</v>
       </c>
@@ -16426,7 +16428,7 @@
         <v>11.052405</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>1002</v>
       </c>
@@ -16455,7 +16457,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>1006</v>
       </c>
@@ -16484,7 +16486,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>1010</v>
       </c>
@@ -16524,7 +16526,7 @@
         <v>78.825308000000007</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>1016</v>
       </c>
@@ -16553,7 +16555,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>1021</v>
       </c>
@@ -16585,7 +16587,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>1025</v>
       </c>
@@ -16614,7 +16616,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>1029</v>
       </c>
@@ -16643,7 +16645,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>1033</v>
       </c>
@@ -16672,7 +16674,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>1037</v>
       </c>
@@ -16701,7 +16703,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>1042</v>
       </c>
@@ -16727,7 +16729,7 @@
         <v>20220414</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>1046</v>
       </c>
@@ -16767,7 +16769,7 @@
         <v>-8.5547679999999993</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>1052</v>
       </c>
@@ -16796,7 +16798,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>1056</v>
       </c>
@@ -16836,7 +16838,7 @@
         <v>-15.891712999999999</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>1061</v>
       </c>
@@ -16865,7 +16867,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>1065</v>
       </c>
@@ -16891,7 +16893,7 @@
         <v>20220713</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>1069</v>
       </c>
@@ -16917,7 +16919,7 @@
         <v>20220901</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>1074</v>
       </c>
@@ -16943,7 +16945,7 @@
         <v>20220504</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>1079</v>
       </c>
@@ -16969,7 +16971,7 @@
         <v>20200902</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>1084</v>
       </c>
@@ -16995,7 +16997,7 @@
         <v>20220822</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>1088</v>
       </c>
@@ -17021,7 +17023,7 @@
         <v>20220704</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>1093</v>
       </c>
@@ -17050,7 +17052,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>1098</v>
       </c>
@@ -17076,7 +17078,7 @@
         <v>20210321</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>1103</v>
       </c>
@@ -17105,7 +17107,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>1108</v>
       </c>
@@ -17137,7 +17139,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>1114</v>
       </c>
@@ -17163,7 +17165,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>1120</v>
       </c>
@@ -17195,7 +17197,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>1126</v>
       </c>
@@ -17227,7 +17229,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>1132</v>
       </c>
@@ -17253,7 +17255,7 @@
         <v>20220915</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>1136</v>
       </c>
@@ -17279,7 +17281,7 @@
         <v>20220831</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>1139</v>
       </c>
@@ -17319,7 +17321,7 @@
         <v>19.278314000000002</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>1145</v>
       </c>
@@ -17351,7 +17353,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>1150</v>
       </c>
@@ -17391,7 +17393,7 @@
         <v>24.662234999999999</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>1155</v>
       </c>
@@ -17420,7 +17422,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>1160</v>
       </c>
@@ -17446,7 +17448,7 @@
         <v>20220328</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>1164</v>
       </c>

</xml_diff>